<commit_message>
International Trade I Notes Update
</commit_message>
<xml_diff>
--- a/2025春课程预选/课程表.xlsx
+++ b/2025春课程预选/课程表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IHEID国际经济学硕士\IHEID\2025春课程预选\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA088E0B-6798-46D4-8191-BA831F74B561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C36F4-C37C-4D99-90F7-ACC8326795C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="23025" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.4"/>
@@ -532,9 +532,6 @@
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="92.25" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -545,6 +542,9 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>